<commit_message>
Querys de CRGs y DPH con prestaciones
</commit_message>
<xml_diff>
--- a/DBA/Reportes BI/2021/Monitoreo CRGs/Prestaciones Nancy.xlsx
+++ b/DBA/Reportes BI/2021/Monitoreo CRGs/Prestaciones Nancy.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\FACOEP\DBA\Reportes BI\2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iachenbach\Gobierno de la Ciudad de Buenos Aires\Pablo Alfredo Gadea - Tablero Facoep P BI\FACOEP\DBA\Reportes BI\2021\Monitoreo CRGs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Grupo</t>
   </si>
   <si>
-    <t>Nancy</t>
-  </si>
-  <si>
     <t>IAC.01</t>
   </si>
   <si>
@@ -44,7 +41,13 @@
     <t>Prestacion</t>
   </si>
   <si>
-    <t>Pablo</t>
+    <t>COV.16</t>
+  </si>
+  <si>
+    <t>COV.17</t>
+  </si>
+  <si>
+    <t>TEST</t>
   </si>
 </sst>
 </file>
@@ -100,8 +103,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:B5" totalsRowShown="0">
-  <autoFilter ref="A1:B5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:B15" totalsRowShown="0">
+  <autoFilter ref="A1:B15"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Prestacion"/>
     <tableColumn id="2" name="Grupo"/>
@@ -373,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,7 +389,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -394,34 +397,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>